<commit_message>
xin loi vi da sua sql :((
Day la lan cuoi thay doi sql :((
</commit_message>
<xml_diff>
--- a/Document/database(exel).xlsx
+++ b/Document/database(exel).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ctnprox-my.sharepoint.com/personal/captain_prox_ctnprox_onmicrosoft_com/Documents/Documents/GitHub/doan1J2School/Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="8_{49CF2EF6-1E6C-485F-9C0C-7DE89611B407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8711467A-5E1C-44F8-80F8-E11C2414556C}"/>
+  <xr:revisionPtr revIDLastSave="126" documentId="8_{49CF2EF6-1E6C-485F-9C0C-7DE89611B407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B9F7B5D-D5D0-4E6B-AC55-8FD2C2B2448A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7E7F7068-F3E1-4B23-8DAA-275A7ED629FC}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7E7F7068-F3E1-4B23-8DAA-275A7ED629FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>id</t>
   </si>
@@ -136,6 +136,24 @@
   </si>
   <si>
     <t>type</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>just note:</t>
+  </si>
+  <si>
+    <t>status name</t>
+  </si>
+  <si>
+    <t>chờ duyệt đơn</t>
+  </si>
+  <si>
+    <t>đã duyệt đơn</t>
+  </si>
+  <si>
+    <t>dã hủy đơn</t>
   </si>
 </sst>
 </file>
@@ -150,7 +168,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,8 +187,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -206,11 +236,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -237,6 +280,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD75231-6A65-4360-9B4A-F43FFFFEEF8B}">
-  <dimension ref="B2:F31"/>
+  <dimension ref="B2:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -760,6 +815,7 @@
       <c r="D26" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F26" s="13"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
@@ -777,6 +833,9 @@
       <c r="B29" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D29" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
@@ -788,7 +847,56 @@
         <v>17</v>
       </c>
     </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D32" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="12"/>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="10">
+        <v>1</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="1">
+        <v>2</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="10">
+        <v>3</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D32:E32"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Edit folder tree, fix(edit employee), add(chart) , fix( database), add (new super admin permission)
Edit folder tree,
fix(edit employee),
fix( database),
add (new super admin permission),
add(chart) ,
</commit_message>
<xml_diff>
--- a/Document/database(exel).xlsx
+++ b/Document/database(exel).xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ctnprox-my.sharepoint.com/personal/captain_prox_ctnprox_onmicrosoft_com/Documents/Documents/GitHub/doan1J2School/Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="126" documentId="8_{49CF2EF6-1E6C-485F-9C0C-7DE89611B407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B9F7B5D-D5D0-4E6B-AC55-8FD2C2B2448A}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="8_{49CF2EF6-1E6C-485F-9C0C-7DE89611B407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C241A62-F5D5-45FC-8897-5944D7E7017B}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7E7F7068-F3E1-4B23-8DAA-275A7ED629FC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7E7F7068-F3E1-4B23-8DAA-275A7ED629FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>id</t>
   </si>
@@ -134,9 +133,6 @@
   </si>
   <si>
     <t>type_id</t>
-  </si>
-  <si>
-    <t>type</t>
   </si>
   <si>
     <t>status</t>
@@ -609,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD75231-6A65-4360-9B4A-F43FFFFEEF8B}">
   <dimension ref="B2:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -642,25 +638,19 @@
       <c r="B5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>33</v>
-      </c>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="D7" s="5"/>
       <c r="F7" s="2" t="s">
         <v>12</v>
       </c>
@@ -835,7 +825,7 @@
         <v>5</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -850,16 +840,16 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D32" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E32" s="13"/>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D33" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.25">
@@ -867,7 +857,7 @@
         <v>1</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.25">
@@ -875,7 +865,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="4:5" x14ac:dyDescent="0.25">
@@ -883,7 +873,7 @@
         <v>3</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="4:5" x14ac:dyDescent="0.25">

</xml_diff>